<commit_message>
Update test file with dependency copy
</commit_message>
<xml_diff>
--- a/tests/fmudesign/data/config/design_input_multiple_dependencies.xlsx
+++ b/tests/fmudesign/data/config/design_input_multiple_dependencies.xlsx
@@ -5,15 +5,16 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="general_input" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="designinput" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="depend1" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="depend2" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="defaultvalues" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="INFO" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="depend3" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="defaultvalues" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="INFO" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="RiskAfterRecalcMacro" vbProcedure="false">""</definedName>
@@ -196,8 +197,32 @@
 </comments>
 </file>
 
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="B2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">If the “to values” in this field are empty, then the “from param” is copied over to the “to param”. In this case NORM3 := copy(NORM2).</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="77">
   <si>
     <t xml:space="preserve">designtype</t>
   </si>
@@ -319,6 +344,9 @@
     <t xml:space="preserve">NORM2</t>
   </si>
   <si>
+    <t xml:space="preserve">depend3</t>
+  </si>
+  <si>
     <t xml:space="preserve">contacts</t>
   </si>
   <si>
@@ -380,6 +408,9 @@
   </si>
   <si>
     <t xml:space="preserve">e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NORM3</t>
   </si>
   <si>
     <t xml:space="preserve">default_value</t>
@@ -761,9 +792,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>360720</xdr:colOff>
+      <xdr:colOff>359280</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>189360</xdr:rowOff>
+      <xdr:rowOff>187920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -773,7 +804,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10045080" cy="9523800"/>
+          <a:ext cx="10056240" cy="9522360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -806,9 +837,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>360720</xdr:colOff>
+      <xdr:colOff>359280</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>189360</xdr:rowOff>
+      <xdr:rowOff>187920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -818,7 +849,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10045080" cy="9523800"/>
+          <a:ext cx="10056240" cy="9522360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -856,9 +887,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>236520</xdr:colOff>
+      <xdr:colOff>235080</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>59760</xdr:rowOff>
+      <xdr:rowOff>58320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -868,7 +899,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10041480" cy="9523800"/>
+          <a:ext cx="10040040" cy="9522360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -901,9 +932,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>236520</xdr:colOff>
+      <xdr:colOff>235080</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>59760</xdr:rowOff>
+      <xdr:rowOff>58320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -913,7 +944,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10041480" cy="9523800"/>
+          <a:ext cx="10040040" cy="9522360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -946,9 +977,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>236520</xdr:colOff>
+      <xdr:colOff>235080</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>59760</xdr:rowOff>
+      <xdr:rowOff>58320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -958,7 +989,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10041480" cy="9523800"/>
+          <a:ext cx="10040040" cy="9522360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -991,9 +1022,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>236520</xdr:colOff>
+      <xdr:colOff>235080</xdr:colOff>
       <xdr:row>54</xdr:row>
-      <xdr:rowOff>59760</xdr:rowOff>
+      <xdr:rowOff>58320</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1003,7 +1034,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="10041480" cy="9523800"/>
+          <a:ext cx="10040040" cy="9522360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1037,11 +1068,11 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10"/>
@@ -1100,11 +1131,11 @@
   </sheetPr>
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J4" activeCellId="0" sqref="J4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q8" activeCellId="0" sqref="Q8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="8.33"/>
@@ -1361,27 +1392,29 @@
       </c>
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
+      <c r="Q7" s="7" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="9" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F8" s="10" t="n">
         <v>1700</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H8" s="10" t="n">
         <v>2700</v>
@@ -1401,7 +1434,7 @@
       <c r="B9" s="10"/>
       <c r="C9" s="12"/>
       <c r="D9" s="9" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="10" t="n">
@@ -1426,7 +1459,7 @@
       <c r="B10" s="10"/>
       <c r="C10" s="12"/>
       <c r="D10" s="9" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="E10" s="13"/>
       <c r="F10" s="10" t="n">
@@ -1448,11 +1481,11 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="9" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="13"/>
@@ -1471,13 +1504,13 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B12" s="8" t="n">
         <v>1</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="8"/>
@@ -1514,11 +1547,11 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.42"/>
@@ -1529,43 +1562,43 @@
         <v>27</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F4" s="16"/>
     </row>
@@ -1587,11 +1620,11 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.42"/>
@@ -1602,10 +1635,10 @@
         <v>35</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1616,7 +1649,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1627,7 +1660,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1638,7 +1671,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F4" s="16"/>
     </row>
@@ -1650,7 +1683,7 @@
         <v>8</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1661,7 +1694,7 @@
         <v>9</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1689,13 +1722,62 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="17"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="18"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="18"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="18"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="18"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="28.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="19" width="12.17"/>
@@ -1707,12 +1789,12 @@
         <v>9</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B2" s="19" t="n">
         <v>1000</v>
@@ -1731,7 +1813,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1760,7 +1842,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="25" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B8" s="19" t="n">
         <v>1700</v>
@@ -1768,7 +1850,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="25" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B9" s="19" t="n">
         <v>1800</v>
@@ -1777,7 +1859,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="25" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B10" s="19" t="n">
         <v>1900</v>
@@ -1787,7 +1869,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B11" s="19" t="n">
         <v>2</v>
@@ -1797,16 +1879,21 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="22"/>
+      <c r="A13" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="19" t="n">
+        <v>-0.5</v>
+      </c>
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
     </row>
@@ -1890,62 +1977,62 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>